<commit_message>
main task is done + added pandas library
done variant 9
added pandas
added xlsx file with currency data
</commit_message>
<xml_diff>
--- a/art/currency.xlsx
+++ b/art/currency.xlsx
@@ -27,7 +27,7 @@
     <t>CNY/RUB</t>
   </si>
   <si>
-    <t>Data</t>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -63,9 +63,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -351,7 +350,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -374,221 +373,221 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>44197</v>
-      </c>
-      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
         <v>68.099999999999994</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>7.8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>44198</v>
-      </c>
-      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
         <v>68.2</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>7.9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>44199</v>
-      </c>
-      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
         <v>68.3</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>44200</v>
-      </c>
-      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
         <v>68.400000000000006</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>7.6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>44201</v>
-      </c>
-      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
         <v>68.5</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>44202</v>
-      </c>
-      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
         <v>68.599999999999994</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>9.3000000000000007</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>44203</v>
-      </c>
-      <c r="B8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
         <v>68.7</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>9.35</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>44204</v>
-      </c>
-      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
         <v>68.8</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>9.6</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>44205</v>
-      </c>
-      <c r="B10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
         <v>68.900000000000006</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>44206</v>
-      </c>
-      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
         <v>69</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>9.9</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>44207</v>
-      </c>
-      <c r="B12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
         <v>68.7</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>10.1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>44208</v>
-      </c>
-      <c r="B13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
         <v>68.5</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>10.199999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>44209</v>
-      </c>
-      <c r="B14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
         <v>68.099999999999994</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>10.1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>44210</v>
-      </c>
-      <c r="B15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
         <v>67.8</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>11.2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>44211</v>
-      </c>
-      <c r="B16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
         <v>69</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>10.8</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>44212</v>
-      </c>
-      <c r="B17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
         <v>70</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>10.7</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>44213</v>
-      </c>
-      <c r="B18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
         <v>73</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>10.9</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>44214</v>
-      </c>
-      <c r="B19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
         <v>72.7</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>9.3000000000000007</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>44215</v>
-      </c>
-      <c r="B20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
         <v>75.400000000000006</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>9.9</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>44216</v>
-      </c>
-      <c r="B21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
         <v>78.599999999999994</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>10.1</v>
       </c>
     </row>

</xml_diff>